<commit_message>
Added Farnah Green pub pedal
</commit_message>
<xml_diff>
--- a/pubrun.xlsx
+++ b/pubrun.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rich\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D829EAF-0900-4AF7-AC43-7E48A4FF77D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9F184F1-F4BC-4586-A544-FF1E862ED990}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="129">
   <si>
     <t>Stanley</t>
   </si>
@@ -408,6 +408,15 @@
   </si>
   <si>
     <t>Very wet, round Elvaston castle ground, past Japanese folly and the weir</t>
+  </si>
+  <si>
+    <t>The Bluebell</t>
+  </si>
+  <si>
+    <t>Farnah Green</t>
+  </si>
+  <si>
+    <t>Pub pedal.</t>
   </si>
 </sst>
 </file>
@@ -817,7 +826,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
+      <selection pane="bottomLeft" activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -959,7 +968,7 @@
         <v>3.4050925925925922E-2</v>
       </c>
       <c r="G6" s="3">
-        <f t="shared" ref="G6:G51" si="1">F6/E6</f>
+        <f t="shared" ref="G6:G52" si="1">F6/E6</f>
         <v>8.3051038843721774E-3</v>
       </c>
       <c r="H6" s="1">
@@ -2860,9 +2869,47 @@
       </c>
     </row>
     <row r="52" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
+      <c r="A52" s="2">
+        <v>43663</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E52" s="1">
+        <v>3.94</v>
+      </c>
+      <c r="F52" s="3">
+        <v>4.5902777777777772E-2</v>
+      </c>
+      <c r="G52" s="3">
+        <f t="shared" si="1"/>
+        <v>1.1650451212633953E-2</v>
+      </c>
+      <c r="H52" s="1">
+        <v>1</v>
+      </c>
+      <c r="I52" s="1">
+        <v>1</v>
+      </c>
+      <c r="J52" s="1">
+        <v>1</v>
+      </c>
+      <c r="N52" s="1">
+        <v>1</v>
+      </c>
+      <c r="O52" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="P52" s="1">
+        <f>SUM(H52:N52)*E52</f>
+        <v>15.76</v>
+      </c>
     </row>
     <row r="53" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
@@ -2879,8 +2926,8 @@
         <v>9.6592945374557888E-3</v>
       </c>
       <c r="H54" s="1">
-        <f>SUM(H5:H51)</f>
-        <v>42</v>
+        <f>SUM(H5:H52)</f>
+        <v>43</v>
       </c>
       <c r="I54" s="1">
         <f t="shared" ref="I54:N54" si="2">SUM(I5:I49)</f>
@@ -2908,7 +2955,7 @@
       </c>
       <c r="P54" s="1">
         <f>SUM(P5:P53)</f>
-        <v>676.73000000000025</v>
+        <v>692.49000000000024</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added Alderwasley and Belper runs
</commit_message>
<xml_diff>
--- a/pubrun.xlsx
+++ b/pubrun.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rich\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9F184F1-F4BC-4586-A544-FF1E862ED990}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09688E55-7928-435E-943C-D0B4565FD752}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15105" yWindow="1155" windowWidth="21090" windowHeight="14565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="134">
   <si>
     <t>Stanley</t>
   </si>
@@ -417,6 +417,21 @@
   </si>
   <si>
     <t>Pub pedal.</t>
+  </si>
+  <si>
+    <t>The Railway / Arkwrights</t>
+  </si>
+  <si>
+    <t>Hilly run, youths lurking in the woods, Limbo frightens a young lady</t>
+  </si>
+  <si>
+    <t>Alderwasley/Belper</t>
+  </si>
+  <si>
+    <t>The Bear / The Green Dragon</t>
+  </si>
+  <si>
+    <t>Slightly lost in the woods. Wizened old landlord</t>
   </si>
 </sst>
 </file>
@@ -822,26 +837,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:P57"/>
+  <dimension ref="A3:P62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A52" sqref="A52"/>
+      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="7.81640625" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.85546875" customWidth="1"/>
     <col min="8" max="14" width="6" customWidth="1"/>
-    <col min="15" max="15" width="54.54296875" customWidth="1"/>
+    <col min="15" max="15" width="54.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:16" s="4" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="4" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -888,7 +903,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -918,7 +933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>41647</v>
       </c>
@@ -948,7 +963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>42144</v>
       </c>
@@ -968,7 +983,7 @@
         <v>3.4050925925925922E-2</v>
       </c>
       <c r="G6" s="3">
-        <f t="shared" ref="G6:G52" si="1">F6/E6</f>
+        <f t="shared" ref="G6:G57" si="1">F6/E6</f>
         <v>8.3051038843721774E-3</v>
       </c>
       <c r="H6" s="1">
@@ -985,7 +1000,7 @@
         <v>12.299999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>42186</v>
       </c>
@@ -1025,7 +1040,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>42291</v>
       </c>
@@ -1065,7 +1080,7 @@
         <v>11.399999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>42319</v>
       </c>
@@ -1111,7 +1126,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>42347</v>
       </c>
@@ -1154,7 +1169,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>42389</v>
       </c>
@@ -1197,7 +1212,7 @@
         <v>21.6</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>42431</v>
       </c>
@@ -1243,7 +1258,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>42452</v>
       </c>
@@ -1283,7 +1298,7 @@
         <v>16.350000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>42480</v>
       </c>
@@ -1329,7 +1344,7 @@
         <v>20.65</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>42508</v>
       </c>
@@ -1372,7 +1387,7 @@
         <v>17.72</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>42536</v>
       </c>
@@ -1415,7 +1430,7 @@
         <v>25.16</v>
       </c>
     </row>
-    <row r="17" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>42564</v>
       </c>
@@ -1458,7 +1473,7 @@
         <v>18.84</v>
       </c>
     </row>
-    <row r="18" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>42577</v>
       </c>
@@ -1498,7 +1513,7 @@
         <v>13.919999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>42592</v>
       </c>
@@ -1538,7 +1553,7 @@
         <v>15.450000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>42641</v>
       </c>
@@ -1578,7 +1593,7 @@
         <v>9.870000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>42655</v>
       </c>
@@ -1621,7 +1636,7 @@
         <v>17.52</v>
       </c>
     </row>
-    <row r="22" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>42671</v>
       </c>
@@ -1661,7 +1676,7 @@
         <v>10.350000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>42690</v>
       </c>
@@ -1707,7 +1722,7 @@
         <v>19.55</v>
       </c>
     </row>
-    <row r="24" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>42718</v>
       </c>
@@ -1750,7 +1765,7 @@
         <v>13.71</v>
       </c>
     </row>
-    <row r="25" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>42760</v>
       </c>
@@ -1790,7 +1805,7 @@
         <v>9.33</v>
       </c>
     </row>
-    <row r="26" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>42781</v>
       </c>
@@ -1833,7 +1848,7 @@
         <v>11.850000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>42809</v>
       </c>
@@ -1876,7 +1891,7 @@
         <v>11.56</v>
       </c>
     </row>
-    <row r="28" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>42844</v>
       </c>
@@ -1913,7 +1928,7 @@
         <v>7.68</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>42865</v>
       </c>
@@ -1956,7 +1971,7 @@
         <v>19.48</v>
       </c>
     </row>
-    <row r="30" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>42879</v>
       </c>
@@ -1999,7 +2014,7 @@
         <v>21.16</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>42907</v>
       </c>
@@ -2036,7 +2051,7 @@
         <v>9.52</v>
       </c>
     </row>
-    <row r="32" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>42920</v>
       </c>
@@ -2082,7 +2097,7 @@
         <v>23.75</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>42956</v>
       </c>
@@ -2122,7 +2137,7 @@
         <v>9.09</v>
       </c>
     </row>
-    <row r="34" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>42991</v>
       </c>
@@ -2165,7 +2180,7 @@
         <v>23.24</v>
       </c>
     </row>
-    <row r="35" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>43033</v>
       </c>
@@ -2208,7 +2223,7 @@
         <v>21.64</v>
       </c>
     </row>
-    <row r="36" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>43061</v>
       </c>
@@ -2248,7 +2263,7 @@
         <v>16.080000000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>43117</v>
       </c>
@@ -2291,7 +2306,7 @@
         <v>22.16</v>
       </c>
     </row>
-    <row r="38" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>43152</v>
       </c>
@@ -2334,7 +2349,7 @@
         <v>17.28</v>
       </c>
     </row>
-    <row r="39" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>43181</v>
       </c>
@@ -2374,7 +2389,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>43216</v>
       </c>
@@ -2420,7 +2435,7 @@
         <v>21.85</v>
       </c>
     </row>
-    <row r="41" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>43244</v>
       </c>
@@ -2460,7 +2475,7 @@
         <v>13.080000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>43272</v>
       </c>
@@ -2503,7 +2518,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="43" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>43354</v>
       </c>
@@ -2543,7 +2558,7 @@
         <v>6.57</v>
       </c>
     </row>
-    <row r="44" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43384</v>
       </c>
@@ -2583,7 +2598,7 @@
         <v>16.350000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>43432</v>
       </c>
@@ -2623,7 +2638,7 @@
         <v>7.86</v>
       </c>
     </row>
-    <row r="46" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>43488</v>
       </c>
@@ -2666,7 +2681,7 @@
         <v>10.28</v>
       </c>
     </row>
-    <row r="47" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>43523</v>
       </c>
@@ -2709,7 +2724,7 @@
         <v>14.84</v>
       </c>
     </row>
-    <row r="48" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>43544</v>
       </c>
@@ -2752,7 +2767,7 @@
         <v>18.96</v>
       </c>
     </row>
-    <row r="49" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>43572</v>
       </c>
@@ -2792,7 +2807,7 @@
         <v>9.69</v>
       </c>
     </row>
-    <row r="50" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
       <c r="B50" s="1" t="s">
         <v>121</v>
@@ -2825,7 +2840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>43628</v>
       </c>
@@ -2868,7 +2883,7 @@
         <v>21.84</v>
       </c>
     </row>
-    <row r="52" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>43663</v>
       </c>
@@ -2911,61 +2926,151 @@
         <v>15.76</v>
       </c>
     </row>
-    <row r="53" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="2"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-    </row>
-    <row r="54" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
+        <v>43705</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E53" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F53" s="3">
+        <v>3.7106481481481483E-2</v>
+      </c>
+      <c r="G53" s="3">
+        <f>F53/E53</f>
+        <v>9.0503613369467047E-3</v>
+      </c>
+      <c r="H53" s="1">
+        <v>1</v>
+      </c>
+      <c r="J53" s="1">
+        <v>1</v>
+      </c>
+      <c r="N53" s="1">
+        <v>1</v>
+      </c>
+      <c r="O53" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="P53" s="1">
+        <f>SUM(H53:N53)*E53</f>
+        <v>12.299999999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
+        <v>43726</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="E54" s="1">
+        <v>3.46</v>
+      </c>
+      <c r="F54" s="3">
+        <v>3.2974537037037038E-2</v>
+      </c>
+      <c r="G54" s="3">
+        <f>F54/E54</f>
+        <v>9.530213016484693E-3</v>
+      </c>
+      <c r="H54" s="1">
+        <v>1</v>
+      </c>
+      <c r="J54" s="1">
+        <v>1</v>
+      </c>
+      <c r="L54" s="1">
+        <v>1</v>
+      </c>
+      <c r="N54" s="1">
+        <v>1</v>
+      </c>
+      <c r="O54" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="P54" s="1">
+        <f>SUM(H54:N54)*E54</f>
+        <v>13.84</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A57" s="2"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+    </row>
+    <row r="58" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A58" s="2"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+    </row>
+    <row r="59" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="E59" s="1">
         <f>SUM(E5:E49)</f>
         <v>183.57</v>
       </c>
-      <c r="G54" s="3">
+      <c r="G59" s="3">
         <f>AVERAGE(G6:G49)</f>
         <v>9.6592945374557888E-3</v>
       </c>
-      <c r="H54" s="1">
+      <c r="H59" s="1">
         <f>SUM(H5:H52)</f>
         <v>43</v>
       </c>
-      <c r="I54" s="1">
-        <f t="shared" ref="I54:N54" si="2">SUM(I5:I49)</f>
+      <c r="I59" s="1">
+        <f t="shared" ref="I59:N59" si="2">SUM(I5:I49)</f>
         <v>29</v>
       </c>
-      <c r="J54" s="1">
+      <c r="J59" s="1">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="K54" s="1">
+      <c r="K59" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L54" s="1">
+      <c r="L59" s="1">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="M54" s="1">
+      <c r="M59" s="1">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="N54" s="1">
+      <c r="N59" s="1">
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="P54" s="1">
-        <f>SUM(P5:P53)</f>
-        <v>692.49000000000024</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="H57" s="1"/>
-      <c r="I57" s="1"/>
-      <c r="J57" s="6"/>
-      <c r="K57" s="6"/>
-      <c r="L57" s="6"/>
-      <c r="M57" s="6"/>
-      <c r="N57" s="6"/>
+      <c r="P59" s="1">
+        <f>SUM(P5:P58)</f>
+        <v>718.63000000000022</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="6"/>
+      <c r="K62" s="6"/>
+      <c r="L62" s="6"/>
+      <c r="M62" s="6"/>
+      <c r="N62" s="6"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:L13">
@@ -2982,7 +3087,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2994,7 +3099,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Wirksworth pub run
</commit_message>
<xml_diff>
--- a/pubrun.xlsx
+++ b/pubrun.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA44359D-BF18-4F10-AF04-D9233109344F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCEDBDD-BE1C-4372-876A-A895854AF724}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="645" yWindow="825" windowWidth="21090" windowHeight="14565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30" yWindow="810" windowWidth="19815" windowHeight="14565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="138">
   <si>
     <t>Stanley</t>
   </si>
@@ -435,6 +437,15 @@
   </si>
   <si>
     <t>Craft ale and wiff waff</t>
+  </si>
+  <si>
+    <t>The Malt Shovel</t>
+  </si>
+  <si>
+    <t>Wirksworth Moor</t>
+  </si>
+  <si>
+    <t>Astronomical observations, Black Rocks</t>
   </si>
 </sst>
 </file>
@@ -840,11 +851,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:P62"/>
+  <dimension ref="A3:P63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O56" sqref="O56"/>
+      <selection pane="bottomLeft" activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2806,7 +2817,7 @@
         <v>120</v>
       </c>
       <c r="P49" s="1">
-        <f t="shared" ref="P49:P55" si="2">SUM(H49:N49)*E49</f>
+        <f t="shared" ref="P49:P56" si="2">SUM(H49:N49)*E49</f>
         <v>9.69</v>
       </c>
     </row>
@@ -3055,67 +3066,107 @@
         <v>14.16</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2"/>
-    <row r="57" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A57" s="2"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-    </row>
+    <row r="56" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
+        <v>43845</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E56" s="1">
+        <v>2.71</v>
+      </c>
+      <c r="F56" s="3">
+        <v>4.08912037037037E-2</v>
+      </c>
+      <c r="G56" s="1">
+        <f>F56/E56</f>
+        <v>1.5089005056717232E-2</v>
+      </c>
+      <c r="H56" s="1">
+        <v>1</v>
+      </c>
+      <c r="J56" s="1">
+        <v>1</v>
+      </c>
+      <c r="N56" s="1">
+        <v>1</v>
+      </c>
+      <c r="O56" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="P56" s="1">
+        <f t="shared" si="2"/>
+        <v>8.129999999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2"/>
     <row r="58" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
     </row>
     <row r="59" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="E59" s="1">
+      <c r="A59" s="2"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+    </row>
+    <row r="60" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="E60" s="1">
         <f>SUM(E5:E49)</f>
         <v>183.57</v>
       </c>
-      <c r="G59" s="3">
+      <c r="G60" s="3">
         <f>AVERAGE(G6:G49)</f>
         <v>9.6592945374557888E-3</v>
       </c>
-      <c r="H59" s="1">
+      <c r="H60" s="1">
         <f>SUM(H5:H52)</f>
         <v>43</v>
       </c>
-      <c r="I59" s="1">
-        <f t="shared" ref="I59:N59" si="3">SUM(I5:I49)</f>
+      <c r="I60" s="1">
+        <f t="shared" ref="I60:N60" si="3">SUM(I5:I49)</f>
         <v>29</v>
       </c>
-      <c r="J59" s="1">
+      <c r="J60" s="1">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="K59" s="1">
+      <c r="K60" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L59" s="1">
+      <c r="L60" s="1">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="M59" s="1">
+      <c r="M60" s="1">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="N59" s="1">
+      <c r="N60" s="1">
         <f t="shared" si="3"/>
         <v>41</v>
       </c>
-      <c r="P59" s="1">
-        <f>SUM(P5:P58)</f>
-        <v>732.79000000000019</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H62" s="1"/>
-      <c r="I62" s="1"/>
-      <c r="J62" s="6"/>
-      <c r="K62" s="6"/>
-      <c r="L62" s="6"/>
-      <c r="M62" s="6"/>
-      <c r="N62" s="6"/>
+      <c r="P60" s="1">
+        <f>SUM(P5:P59)</f>
+        <v>740.92000000000019</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="6"/>
+      <c r="K63" s="6"/>
+      <c r="L63" s="6"/>
+      <c r="M63" s="6"/>
+      <c r="N63" s="6"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:L13">

</xml_diff>

<commit_message>
Added Jug of Wine run
</commit_message>
<xml_diff>
--- a/pubrun.xlsx
+++ b/pubrun.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCEDBDD-BE1C-4372-876A-A895854AF724}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7310264-0026-4C79-9AAC-FAE927CEDB62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="810" windowWidth="19815" windowHeight="14565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="1155" windowWidth="19815" windowHeight="14565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="141">
   <si>
     <t>Stanley</t>
   </si>
@@ -446,6 +446,15 @@
   </si>
   <si>
     <t>Astronomical observations, Black Rocks</t>
+  </si>
+  <si>
+    <t>The Jug of Wine</t>
+  </si>
+  <si>
+    <t>Lea</t>
+  </si>
+  <si>
+    <t>Trespass, "Oi, where you going?", charming old church</t>
   </si>
 </sst>
 </file>
@@ -855,7 +864,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A56" sqref="A56"/>
+      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2817,7 +2826,7 @@
         <v>120</v>
       </c>
       <c r="P49" s="1">
-        <f t="shared" ref="P49:P56" si="2">SUM(H49:N49)*E49</f>
+        <f t="shared" ref="P49:P57" si="2">SUM(H49:N49)*E49</f>
         <v>9.69</v>
       </c>
     </row>
@@ -3106,7 +3115,49 @@
         <v>8.129999999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
+        <v>43887</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" s="1">
+        <v>3.82</v>
+      </c>
+      <c r="F57" s="3">
+        <v>4.2361111111111106E-2</v>
+      </c>
+      <c r="G57" s="1">
+        <f>F57/E57</f>
+        <v>1.1089296102385108E-2</v>
+      </c>
+      <c r="H57" s="1">
+        <v>1</v>
+      </c>
+      <c r="J57" s="1">
+        <v>1</v>
+      </c>
+      <c r="L57" s="1">
+        <v>1</v>
+      </c>
+      <c r="N57" s="1">
+        <v>1</v>
+      </c>
+      <c r="O57" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="P57" s="1">
+        <f t="shared" si="2"/>
+        <v>15.28</v>
+      </c>
+    </row>
     <row r="58" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
       <c r="F58" s="3"/>
@@ -3156,7 +3207,7 @@
       </c>
       <c r="P60" s="1">
         <f>SUM(P5:P59)</f>
-        <v>740.92000000000019</v>
+        <v>756.20000000000016</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
White Hart details added
</commit_message>
<xml_diff>
--- a/pubrun.xlsx
+++ b/pubrun.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rich\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7310264-0026-4C79-9AAC-FAE927CEDB62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D56FC41-B413-4D3E-8622-D61B41C454BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="1155" windowWidth="19815" windowHeight="14565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="146">
   <si>
     <t>Stanley</t>
   </si>
@@ -455,6 +455,21 @@
   </si>
   <si>
     <t>Trespass, "Oi, where you going?", charming old church</t>
+  </si>
+  <si>
+    <t>Bargates</t>
+  </si>
+  <si>
+    <t>Zoom</t>
+  </si>
+  <si>
+    <t>virtual</t>
+  </si>
+  <si>
+    <t>Lockdown virtual catch-up</t>
+  </si>
+  <si>
+    <t>Socially distanced</t>
   </si>
 </sst>
 </file>
@@ -860,26 +875,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:P63"/>
+  <dimension ref="A3:P64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
+      <pane ySplit="3" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="7.85546875" customWidth="1"/>
+    <col min="5" max="5" width="5.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.81640625" customWidth="1"/>
     <col min="8" max="14" width="6" customWidth="1"/>
-    <col min="15" max="15" width="54.5703125" customWidth="1"/>
+    <col min="15" max="15" width="54.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:16" s="4" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" s="4" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -926,7 +941,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -956,7 +971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>41647</v>
       </c>
@@ -986,7 +1001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>42144</v>
       </c>
@@ -1023,7 +1038,7 @@
         <v>12.299999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>42186</v>
       </c>
@@ -1063,7 +1078,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>42291</v>
       </c>
@@ -1103,7 +1118,7 @@
         <v>11.399999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>42319</v>
       </c>
@@ -1149,7 +1164,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>42347</v>
       </c>
@@ -1192,7 +1207,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>42389</v>
       </c>
@@ -1235,7 +1250,7 @@
         <v>21.6</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>42431</v>
       </c>
@@ -1281,7 +1296,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>42452</v>
       </c>
@@ -1321,7 +1336,7 @@
         <v>16.350000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>42480</v>
       </c>
@@ -1367,7 +1382,7 @@
         <v>20.65</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>42508</v>
       </c>
@@ -1410,7 +1425,7 @@
         <v>17.72</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>42536</v>
       </c>
@@ -1453,7 +1468,7 @@
         <v>25.16</v>
       </c>
     </row>
-    <row r="17" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>42564</v>
       </c>
@@ -1496,7 +1511,7 @@
         <v>18.84</v>
       </c>
     </row>
-    <row r="18" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>42577</v>
       </c>
@@ -1536,7 +1551,7 @@
         <v>13.919999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>42592</v>
       </c>
@@ -1576,7 +1591,7 @@
         <v>15.450000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>42641</v>
       </c>
@@ -1616,7 +1631,7 @@
         <v>9.870000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>42655</v>
       </c>
@@ -1659,7 +1674,7 @@
         <v>17.52</v>
       </c>
     </row>
-    <row r="22" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>42671</v>
       </c>
@@ -1699,7 +1714,7 @@
         <v>10.350000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>42690</v>
       </c>
@@ -1745,7 +1760,7 @@
         <v>19.55</v>
       </c>
     </row>
-    <row r="24" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>42718</v>
       </c>
@@ -1788,7 +1803,7 @@
         <v>13.71</v>
       </c>
     </row>
-    <row r="25" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>42760</v>
       </c>
@@ -1828,7 +1843,7 @@
         <v>9.33</v>
       </c>
     </row>
-    <row r="26" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>42781</v>
       </c>
@@ -1871,7 +1886,7 @@
         <v>11.850000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>42809</v>
       </c>
@@ -1914,7 +1929,7 @@
         <v>11.56</v>
       </c>
     </row>
-    <row r="28" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>42844</v>
       </c>
@@ -1951,7 +1966,7 @@
         <v>7.68</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>42865</v>
       </c>
@@ -1994,7 +2009,7 @@
         <v>19.48</v>
       </c>
     </row>
-    <row r="30" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>42879</v>
       </c>
@@ -2037,7 +2052,7 @@
         <v>21.16</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>42907</v>
       </c>
@@ -2074,7 +2089,7 @@
         <v>9.52</v>
       </c>
     </row>
-    <row r="32" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>42920</v>
       </c>
@@ -2120,7 +2135,7 @@
         <v>23.75</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>42956</v>
       </c>
@@ -2160,7 +2175,7 @@
         <v>9.09</v>
       </c>
     </row>
-    <row r="34" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>42991</v>
       </c>
@@ -2203,7 +2218,7 @@
         <v>23.24</v>
       </c>
     </row>
-    <row r="35" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>43033</v>
       </c>
@@ -2246,7 +2261,7 @@
         <v>21.64</v>
       </c>
     </row>
-    <row r="36" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>43061</v>
       </c>
@@ -2286,7 +2301,7 @@
         <v>16.080000000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>43117</v>
       </c>
@@ -2329,7 +2344,7 @@
         <v>22.16</v>
       </c>
     </row>
-    <row r="38" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>43152</v>
       </c>
@@ -2372,7 +2387,7 @@
         <v>17.28</v>
       </c>
     </row>
-    <row r="39" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>43181</v>
       </c>
@@ -2412,7 +2427,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>43216</v>
       </c>
@@ -2458,7 +2473,7 @@
         <v>21.85</v>
       </c>
     </row>
-    <row r="41" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>43244</v>
       </c>
@@ -2498,7 +2513,7 @@
         <v>13.080000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>43272</v>
       </c>
@@ -2541,7 +2556,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="43" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>43354</v>
       </c>
@@ -2581,7 +2596,7 @@
         <v>6.57</v>
       </c>
     </row>
-    <row r="44" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43384</v>
       </c>
@@ -2621,7 +2636,7 @@
         <v>16.350000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>43432</v>
       </c>
@@ -2661,7 +2676,7 @@
         <v>7.86</v>
       </c>
     </row>
-    <row r="46" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>43488</v>
       </c>
@@ -2704,7 +2719,7 @@
         <v>10.28</v>
       </c>
     </row>
-    <row r="47" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>43523</v>
       </c>
@@ -2747,7 +2762,7 @@
         <v>14.84</v>
       </c>
     </row>
-    <row r="48" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>43544</v>
       </c>
@@ -2790,7 +2805,7 @@
         <v>18.96</v>
       </c>
     </row>
-    <row r="49" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>43572</v>
       </c>
@@ -2826,11 +2841,11 @@
         <v>120</v>
       </c>
       <c r="P49" s="1">
-        <f t="shared" ref="P49:P57" si="2">SUM(H49:N49)*E49</f>
+        <f t="shared" ref="P49:P59" si="2">SUM(H49:N49)*E49</f>
         <v>9.69</v>
       </c>
     </row>
-    <row r="50" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="1" t="s">
         <v>121</v>
@@ -2863,7 +2878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>43628</v>
       </c>
@@ -2906,7 +2921,7 @@
         <v>21.84</v>
       </c>
     </row>
-    <row r="52" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>43663</v>
       </c>
@@ -2949,7 +2964,7 @@
         <v>15.76</v>
       </c>
     </row>
-    <row r="53" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>43705</v>
       </c>
@@ -2989,7 +3004,7 @@
         <v>12.299999999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>43726</v>
       </c>
@@ -3032,7 +3047,7 @@
         <v>13.84</v>
       </c>
     </row>
-    <row r="55" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>43754</v>
       </c>
@@ -3075,7 +3090,7 @@
         <v>14.16</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>43845</v>
       </c>
@@ -3115,7 +3130,7 @@
         <v>8.129999999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>43887</v>
       </c>
@@ -3158,66 +3173,136 @@
         <v>15.28</v>
       </c>
     </row>
-    <row r="58" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A58" s="2"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-    </row>
-    <row r="59" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A59" s="2"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-    </row>
-    <row r="60" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="E60" s="1">
-        <f>SUM(E5:E49)</f>
-        <v>183.57</v>
-      </c>
-      <c r="G60" s="3">
-        <f>AVERAGE(G6:G49)</f>
-        <v>9.6592945374557888E-3</v>
-      </c>
-      <c r="H60" s="1">
-        <f>SUM(H5:H52)</f>
-        <v>43</v>
-      </c>
-      <c r="I60" s="1">
-        <f t="shared" ref="I60:N60" si="3">SUM(I5:I49)</f>
-        <v>29</v>
-      </c>
-      <c r="J60" s="1">
-        <f t="shared" si="3"/>
-        <v>40</v>
-      </c>
-      <c r="K60" s="1">
-        <f t="shared" si="3"/>
+    <row r="58" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F58" s="3">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="H58" s="1">
+        <v>1</v>
+      </c>
+      <c r="I58" s="1">
+        <v>1</v>
+      </c>
+      <c r="J58" s="1">
+        <v>1</v>
+      </c>
+      <c r="N58" s="1">
+        <v>1</v>
+      </c>
+      <c r="O58" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="P58" s="1">
         <v>0</v>
       </c>
-      <c r="L60" s="1">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="M60" s="1">
-        <f t="shared" si="3"/>
+    </row>
+    <row r="59" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>44062</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E59" s="1">
+        <v>3.37</v>
+      </c>
+      <c r="F59" s="3">
+        <v>3.636574074074074E-2</v>
+      </c>
+      <c r="G59" s="3">
+        <f>F59/E59</f>
+        <v>1.0791020991317726E-2</v>
+      </c>
+      <c r="H59" s="1">
+        <v>1</v>
+      </c>
+      <c r="I59" s="1">
+        <v>1</v>
+      </c>
+      <c r="N59" s="1">
+        <v>1</v>
+      </c>
+      <c r="O59" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="P59" s="1">
+        <f t="shared" si="2"/>
+        <v>10.11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+    </row>
+    <row r="61" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+      <c r="E61" s="1">
+        <f>SUM(E5:E59)</f>
+        <v>213.97</v>
+      </c>
+      <c r="G61" s="3">
+        <f>AVERAGE(G6:G59)</f>
+        <v>9.8056799560196119E-3</v>
+      </c>
+      <c r="H61" s="1">
+        <f>SUM(H5:H59)</f>
+        <v>49</v>
+      </c>
+      <c r="I61" s="1">
+        <f>SUM(I5:I59)</f>
+        <v>34</v>
+      </c>
+      <c r="J61" s="1">
+        <f>SUM(J5:J59)</f>
+        <v>49</v>
+      </c>
+      <c r="K61" s="1">
+        <f>SUM(K5:K59)</f>
+        <v>0</v>
+      </c>
+      <c r="L61" s="1">
+        <f>SUM(L5:L59)</f>
+        <v>8</v>
+      </c>
+      <c r="M61" s="1">
+        <f>SUM(M5:M59)</f>
         <v>4</v>
       </c>
-      <c r="N60" s="1">
-        <f t="shared" si="3"/>
-        <v>41</v>
-      </c>
-      <c r="P60" s="1">
-        <f>SUM(P5:P59)</f>
-        <v>756.20000000000016</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
-      <c r="J63" s="6"/>
-      <c r="K63" s="6"/>
-      <c r="L63" s="6"/>
-      <c r="M63" s="6"/>
-      <c r="N63" s="6"/>
+      <c r="N61" s="1">
+        <f>SUM(N5:N59)</f>
+        <v>50</v>
+      </c>
+      <c r="P61" s="1">
+        <f>SUM(P5:P60)</f>
+        <v>766.31000000000017</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="6"/>
+      <c r="K64" s="6"/>
+      <c r="L64" s="6"/>
+      <c r="M64" s="6"/>
+      <c r="N64" s="6"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:L13">
@@ -3234,7 +3319,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3246,7 +3331,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added White Hart, Duffield details
</commit_message>
<xml_diff>
--- a/pubrun.xlsx
+++ b/pubrun.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rich\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Users\richa\Documents\root\activities\fitness\pubrunner.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D56FC41-B413-4D3E-8622-D61B41C454BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E54618-D3DB-4744-956E-427DFA5411EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="147">
   <si>
     <t>Stanley</t>
   </si>
@@ -470,6 +468,9 @@
   </si>
   <si>
     <t>Socially distanced</t>
+  </si>
+  <si>
+    <t>Windley moated manorial complex</t>
   </si>
 </sst>
 </file>
@@ -875,11 +876,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:P64"/>
+  <dimension ref="A3:P65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G60" sqref="G60"/>
+      <selection pane="bottomLeft" activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2841,7 +2842,7 @@
         <v>120</v>
       </c>
       <c r="P49" s="1">
-        <f t="shared" ref="P49:P59" si="2">SUM(H49:N49)*E49</f>
+        <f t="shared" ref="P49:P60" si="2">SUM(H49:N49)*E49</f>
         <v>9.69</v>
       </c>
     </row>
@@ -3249,60 +3250,100 @@
       </c>
     </row>
     <row r="60" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="2"/>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
+      <c r="A60" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E60" s="1">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="F60" s="3">
+        <v>4.3784722222222218E-2</v>
+      </c>
+      <c r="G60" s="3">
+        <f>F60/E60</f>
+        <v>1.057601986044015E-2</v>
+      </c>
+      <c r="H60" s="1">
+        <v>1</v>
+      </c>
+      <c r="J60" s="1">
+        <v>1</v>
+      </c>
+      <c r="N60" s="1">
+        <v>1</v>
+      </c>
+      <c r="O60" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="P60" s="1">
+        <f t="shared" si="2"/>
+        <v>12.419999999999998</v>
+      </c>
     </row>
     <row r="61" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
-      <c r="E61" s="1">
-        <f>SUM(E5:E59)</f>
-        <v>213.97</v>
-      </c>
-      <c r="G61" s="3">
-        <f>AVERAGE(G6:G59)</f>
-        <v>9.8056799560196119E-3</v>
-      </c>
-      <c r="H61" s="1">
-        <f>SUM(H5:H59)</f>
+      <c r="A61" s="2"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+    </row>
+    <row r="62" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+      <c r="E62" s="1">
+        <f>SUM(E5:E60)</f>
+        <v>218.10999999999999</v>
+      </c>
+      <c r="G62" s="3">
+        <f>AVERAGE(G6:G60)</f>
+        <v>9.8202146711973571E-3</v>
+      </c>
+      <c r="H62" s="1">
+        <f>SUM(H5:H60)</f>
+        <v>50</v>
+      </c>
+      <c r="I62" s="1">
+        <f t="shared" ref="H62:N62" si="3">SUM(I5:I59)</f>
+        <v>34</v>
+      </c>
+      <c r="J62" s="1">
+        <f t="shared" si="3"/>
         <v>49</v>
       </c>
-      <c r="I61" s="1">
-        <f>SUM(I5:I59)</f>
-        <v>34</v>
-      </c>
-      <c r="J61" s="1">
-        <f>SUM(J5:J59)</f>
-        <v>49</v>
-      </c>
-      <c r="K61" s="1">
-        <f>SUM(K5:K59)</f>
+      <c r="K62" s="1">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L61" s="1">
-        <f>SUM(L5:L59)</f>
+      <c r="L62" s="1">
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="M61" s="1">
-        <f>SUM(M5:M59)</f>
+      <c r="M62" s="1">
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="N61" s="1">
-        <f>SUM(N5:N59)</f>
-        <v>50</v>
-      </c>
-      <c r="P61" s="1">
-        <f>SUM(P5:P60)</f>
-        <v>766.31000000000017</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
-      <c r="J64" s="6"/>
-      <c r="K64" s="6"/>
-      <c r="L64" s="6"/>
-      <c r="M64" s="6"/>
-      <c r="N64" s="6"/>
+      <c r="N62" s="1">
+        <f>SUM(N5:N60)</f>
+        <v>51</v>
+      </c>
+      <c r="P62" s="1">
+        <f>SUM(P5:P61)</f>
+        <v>778.73000000000013</v>
+      </c>
+    </row>
+    <row r="65" spans="8:14" x14ac:dyDescent="0.35">
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="6"/>
+      <c r="K65" s="6"/>
+      <c r="L65" s="6"/>
+      <c r="M65" s="6"/>
+      <c r="N65" s="6"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:L13">
@@ -3311,28 +3352,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added last 2 runs
</commit_message>
<xml_diff>
--- a/pubrun.xlsx
+++ b/pubrun.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Users\richa\Documents\root\activities\fitness\pubrunner.github.io\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Documents\root\activities\fitness\pubrunner.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E54618-D3DB-4744-956E-427DFA5411EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DABC27B-2E97-4BD1-95A9-78A6486846D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16680" yWindow="585" windowWidth="15840" windowHeight="14640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="149">
   <si>
     <t>Stanley</t>
   </si>
@@ -471,6 +471,12 @@
   </si>
   <si>
     <t>Windley moated manorial complex</t>
+  </si>
+  <si>
+    <t>Back after lockdown</t>
+  </si>
+  <si>
+    <t>A gentle trot to Makeney and back</t>
   </si>
 </sst>
 </file>
@@ -876,26 +882,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:P65"/>
+  <dimension ref="A3:P67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A60" sqref="A60"/>
+      <pane ySplit="3" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="7.81640625" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.85546875" customWidth="1"/>
     <col min="8" max="14" width="6" customWidth="1"/>
-    <col min="15" max="15" width="54.54296875" customWidth="1"/>
+    <col min="15" max="15" width="54.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:16" s="4" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="4" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -942,7 +948,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -972,7 +978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>41647</v>
       </c>
@@ -1002,7 +1008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>42144</v>
       </c>
@@ -1039,7 +1045,7 @@
         <v>12.299999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>42186</v>
       </c>
@@ -1079,7 +1085,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>42291</v>
       </c>
@@ -1119,7 +1125,7 @@
         <v>11.399999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>42319</v>
       </c>
@@ -1165,7 +1171,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>42347</v>
       </c>
@@ -1208,7 +1214,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>42389</v>
       </c>
@@ -1251,7 +1257,7 @@
         <v>21.6</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>42431</v>
       </c>
@@ -1297,7 +1303,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>42452</v>
       </c>
@@ -1337,7 +1343,7 @@
         <v>16.350000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>42480</v>
       </c>
@@ -1383,7 +1389,7 @@
         <v>20.65</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>42508</v>
       </c>
@@ -1426,7 +1432,7 @@
         <v>17.72</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>42536</v>
       </c>
@@ -1469,7 +1475,7 @@
         <v>25.16</v>
       </c>
     </row>
-    <row r="17" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>42564</v>
       </c>
@@ -1512,7 +1518,7 @@
         <v>18.84</v>
       </c>
     </row>
-    <row r="18" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>42577</v>
       </c>
@@ -1552,7 +1558,7 @@
         <v>13.919999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>42592</v>
       </c>
@@ -1592,7 +1598,7 @@
         <v>15.450000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>42641</v>
       </c>
@@ -1632,7 +1638,7 @@
         <v>9.870000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>42655</v>
       </c>
@@ -1675,7 +1681,7 @@
         <v>17.52</v>
       </c>
     </row>
-    <row r="22" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>42671</v>
       </c>
@@ -1715,7 +1721,7 @@
         <v>10.350000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>42690</v>
       </c>
@@ -1761,7 +1767,7 @@
         <v>19.55</v>
       </c>
     </row>
-    <row r="24" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>42718</v>
       </c>
@@ -1804,7 +1810,7 @@
         <v>13.71</v>
       </c>
     </row>
-    <row r="25" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>42760</v>
       </c>
@@ -1844,7 +1850,7 @@
         <v>9.33</v>
       </c>
     </row>
-    <row r="26" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>42781</v>
       </c>
@@ -1887,7 +1893,7 @@
         <v>11.850000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>42809</v>
       </c>
@@ -1930,7 +1936,7 @@
         <v>11.56</v>
       </c>
     </row>
-    <row r="28" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>42844</v>
       </c>
@@ -1967,7 +1973,7 @@
         <v>7.68</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>42865</v>
       </c>
@@ -2010,7 +2016,7 @@
         <v>19.48</v>
       </c>
     </row>
-    <row r="30" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>42879</v>
       </c>
@@ -2053,7 +2059,7 @@
         <v>21.16</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>42907</v>
       </c>
@@ -2090,7 +2096,7 @@
         <v>9.52</v>
       </c>
     </row>
-    <row r="32" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>42920</v>
       </c>
@@ -2136,7 +2142,7 @@
         <v>23.75</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>42956</v>
       </c>
@@ -2176,7 +2182,7 @@
         <v>9.09</v>
       </c>
     </row>
-    <row r="34" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>42991</v>
       </c>
@@ -2219,7 +2225,7 @@
         <v>23.24</v>
       </c>
     </row>
-    <row r="35" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>43033</v>
       </c>
@@ -2262,7 +2268,7 @@
         <v>21.64</v>
       </c>
     </row>
-    <row r="36" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>43061</v>
       </c>
@@ -2302,7 +2308,7 @@
         <v>16.080000000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>43117</v>
       </c>
@@ -2345,7 +2351,7 @@
         <v>22.16</v>
       </c>
     </row>
-    <row r="38" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>43152</v>
       </c>
@@ -2388,7 +2394,7 @@
         <v>17.28</v>
       </c>
     </row>
-    <row r="39" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>43181</v>
       </c>
@@ -2428,7 +2434,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>43216</v>
       </c>
@@ -2474,7 +2480,7 @@
         <v>21.85</v>
       </c>
     </row>
-    <row r="41" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>43244</v>
       </c>
@@ -2514,7 +2520,7 @@
         <v>13.080000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>43272</v>
       </c>
@@ -2557,7 +2563,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="43" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>43354</v>
       </c>
@@ -2597,7 +2603,7 @@
         <v>6.57</v>
       </c>
     </row>
-    <row r="44" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43384</v>
       </c>
@@ -2637,7 +2643,7 @@
         <v>16.350000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>43432</v>
       </c>
@@ -2677,7 +2683,7 @@
         <v>7.86</v>
       </c>
     </row>
-    <row r="46" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>43488</v>
       </c>
@@ -2720,7 +2726,7 @@
         <v>10.28</v>
       </c>
     </row>
-    <row r="47" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>43523</v>
       </c>
@@ -2763,7 +2769,7 @@
         <v>14.84</v>
       </c>
     </row>
-    <row r="48" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>43544</v>
       </c>
@@ -2806,7 +2812,7 @@
         <v>18.96</v>
       </c>
     </row>
-    <row r="49" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>43572</v>
       </c>
@@ -2842,11 +2848,11 @@
         <v>120</v>
       </c>
       <c r="P49" s="1">
-        <f t="shared" ref="P49:P60" si="2">SUM(H49:N49)*E49</f>
+        <f t="shared" ref="P49:P62" si="2">SUM(H49:N49)*E49</f>
         <v>9.69</v>
       </c>
     </row>
-    <row r="50" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
       <c r="B50" s="1" t="s">
         <v>121</v>
@@ -2879,7 +2885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>43628</v>
       </c>
@@ -2922,7 +2928,7 @@
         <v>21.84</v>
       </c>
     </row>
-    <row r="52" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>43663</v>
       </c>
@@ -2965,7 +2971,7 @@
         <v>15.76</v>
       </c>
     </row>
-    <row r="53" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>43705</v>
       </c>
@@ -3005,7 +3011,7 @@
         <v>12.299999999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>43726</v>
       </c>
@@ -3048,7 +3054,7 @@
         <v>13.84</v>
       </c>
     </row>
-    <row r="55" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>43754</v>
       </c>
@@ -3091,7 +3097,7 @@
         <v>14.16</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>43845</v>
       </c>
@@ -3131,7 +3137,7 @@
         <v>8.129999999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>43887</v>
       </c>
@@ -3174,7 +3180,7 @@
         <v>15.28</v>
       </c>
     </row>
-    <row r="58" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>44013</v>
       </c>
@@ -3209,7 +3215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>44062</v>
       </c>
@@ -3249,7 +3255,7 @@
         <v>10.11</v>
       </c>
     </row>
-    <row r="60" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>44097</v>
       </c>
@@ -3289,61 +3295,144 @@
         <v>12.419999999999998</v>
       </c>
     </row>
-    <row r="61" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="2"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
-    </row>
-    <row r="62" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A61" s="2">
+        <v>44307</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E61" s="1">
+        <v>1.72</v>
+      </c>
+      <c r="F61" s="3">
+        <v>2.0219907407407409E-2</v>
+      </c>
+      <c r="G61" s="3">
+        <f>F61/E61</f>
+        <v>1.1755760120585703E-2</v>
+      </c>
+      <c r="H61" s="1">
+        <v>1</v>
+      </c>
+      <c r="I61" s="1">
+        <v>1</v>
+      </c>
+      <c r="J61" s="1">
+        <v>1</v>
+      </c>
+      <c r="N61" s="1">
+        <v>1</v>
+      </c>
+      <c r="O61" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="P61" s="1">
+        <f t="shared" si="2"/>
+        <v>6.88</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A62" s="2">
+        <v>44335</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="E62" s="1">
-        <f>SUM(E5:E60)</f>
-        <v>218.10999999999999</v>
+        <v>2.33</v>
+      </c>
+      <c r="F62" s="3">
+        <v>2.3738425925925923E-2</v>
       </c>
       <c r="G62" s="3">
-        <f>AVERAGE(G6:G60)</f>
-        <v>9.8202146711973571E-3</v>
+        <f>F62/E62</f>
+        <v>1.0188165633444601E-2</v>
       </c>
       <c r="H62" s="1">
-        <f>SUM(H5:H60)</f>
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="I62" s="1">
-        <f t="shared" ref="H62:N62" si="3">SUM(I5:I59)</f>
+        <v>1</v>
+      </c>
+      <c r="N62" s="1">
+        <v>1</v>
+      </c>
+      <c r="O62" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="P62" s="1">
+        <f t="shared" si="2"/>
+        <v>6.99</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A63" s="2"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+    </row>
+    <row r="64" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="E64" s="1">
+        <f>SUM(E5:E62)</f>
+        <v>222.16</v>
+      </c>
+      <c r="G64" s="3">
+        <f>AVERAGE(G6:G62)</f>
+        <v>9.8620964241361853E-3</v>
+      </c>
+      <c r="H64" s="1">
+        <f>SUM(H5:H62)</f>
+        <v>52</v>
+      </c>
+      <c r="I64" s="1">
+        <f t="shared" ref="I64:M64" si="3">SUM(I5:I59)</f>
         <v>34</v>
       </c>
-      <c r="J62" s="1">
+      <c r="J64" s="1">
         <f t="shared" si="3"/>
         <v>49</v>
       </c>
-      <c r="K62" s="1">
+      <c r="K64" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L62" s="1">
+      <c r="L64" s="1">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="M62" s="1">
+      <c r="M64" s="1">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="N62" s="1">
-        <f>SUM(N5:N60)</f>
-        <v>51</v>
-      </c>
-      <c r="P62" s="1">
-        <f>SUM(P5:P61)</f>
-        <v>778.73000000000013</v>
-      </c>
-    </row>
-    <row r="65" spans="8:14" x14ac:dyDescent="0.35">
-      <c r="H65" s="1"/>
-      <c r="I65" s="1"/>
-      <c r="J65" s="6"/>
-      <c r="K65" s="6"/>
-      <c r="L65" s="6"/>
-      <c r="M65" s="6"/>
-      <c r="N65" s="6"/>
+      <c r="N64" s="1">
+        <f>SUM(N5:N62)</f>
+        <v>53</v>
+      </c>
+      <c r="P64" s="1">
+        <f>SUM(P5:P63)</f>
+        <v>792.60000000000014</v>
+      </c>
+    </row>
+    <row r="67" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="6"/>
+      <c r="K67" s="6"/>
+      <c r="L67" s="6"/>
+      <c r="M67" s="6"/>
+      <c r="N67" s="6"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:L13">

</xml_diff>

<commit_message>
Spotted Cow and Wollaton pub runs added
</commit_message>
<xml_diff>
--- a/pubrun.xlsx
+++ b/pubrun.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Documents\root\activities\fitness\pubrunner.github.io\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rich\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DABC27B-2E97-4BD1-95A9-78A6486846D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA62C2C-B070-4C4C-9996-CA407CA3F662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16680" yWindow="585" windowWidth="15840" windowHeight="14640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="155">
   <si>
     <t>Stanley</t>
   </si>
@@ -477,6 +477,24 @@
   </si>
   <si>
     <t>A gentle trot to Makeney and back</t>
+  </si>
+  <si>
+    <t>The Admiral Rodney</t>
+  </si>
+  <si>
+    <t>Wollaton</t>
+  </si>
+  <si>
+    <t>Bicycle repair man</t>
+  </si>
+  <si>
+    <t>Darley Abbey</t>
+  </si>
+  <si>
+    <t>The Shed / The Furnace</t>
+  </si>
+  <si>
+    <t>Lost in the nature reserve, highland cattle</t>
   </si>
 </sst>
 </file>
@@ -882,26 +900,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:P67"/>
+  <dimension ref="A3:P69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A62" sqref="A62"/>
+      <pane ySplit="3" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="7.85546875" customWidth="1"/>
+    <col min="5" max="5" width="5.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.81640625" customWidth="1"/>
     <col min="8" max="14" width="6" customWidth="1"/>
-    <col min="15" max="15" width="54.5703125" customWidth="1"/>
+    <col min="15" max="15" width="54.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:16" s="4" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" s="4" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -948,7 +966,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -978,7 +996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>41647</v>
       </c>
@@ -1008,7 +1026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>42144</v>
       </c>
@@ -1045,7 +1063,7 @@
         <v>12.299999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>42186</v>
       </c>
@@ -1085,7 +1103,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>42291</v>
       </c>
@@ -1125,7 +1143,7 @@
         <v>11.399999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>42319</v>
       </c>
@@ -1171,7 +1189,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>42347</v>
       </c>
@@ -1214,7 +1232,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>42389</v>
       </c>
@@ -1257,7 +1275,7 @@
         <v>21.6</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>42431</v>
       </c>
@@ -1303,7 +1321,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>42452</v>
       </c>
@@ -1343,7 +1361,7 @@
         <v>16.350000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>42480</v>
       </c>
@@ -1389,7 +1407,7 @@
         <v>20.65</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>42508</v>
       </c>
@@ -1432,7 +1450,7 @@
         <v>17.72</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>42536</v>
       </c>
@@ -1475,7 +1493,7 @@
         <v>25.16</v>
       </c>
     </row>
-    <row r="17" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>42564</v>
       </c>
@@ -1518,7 +1536,7 @@
         <v>18.84</v>
       </c>
     </row>
-    <row r="18" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>42577</v>
       </c>
@@ -1558,7 +1576,7 @@
         <v>13.919999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>42592</v>
       </c>
@@ -1598,7 +1616,7 @@
         <v>15.450000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>42641</v>
       </c>
@@ -1638,7 +1656,7 @@
         <v>9.870000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>42655</v>
       </c>
@@ -1681,7 +1699,7 @@
         <v>17.52</v>
       </c>
     </row>
-    <row r="22" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>42671</v>
       </c>
@@ -1721,7 +1739,7 @@
         <v>10.350000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>42690</v>
       </c>
@@ -1767,7 +1785,7 @@
         <v>19.55</v>
       </c>
     </row>
-    <row r="24" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>42718</v>
       </c>
@@ -1810,7 +1828,7 @@
         <v>13.71</v>
       </c>
     </row>
-    <row r="25" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>42760</v>
       </c>
@@ -1850,7 +1868,7 @@
         <v>9.33</v>
       </c>
     </row>
-    <row r="26" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>42781</v>
       </c>
@@ -1893,7 +1911,7 @@
         <v>11.850000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>42809</v>
       </c>
@@ -1936,7 +1954,7 @@
         <v>11.56</v>
       </c>
     </row>
-    <row r="28" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>42844</v>
       </c>
@@ -1973,7 +1991,7 @@
         <v>7.68</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>42865</v>
       </c>
@@ -2016,7 +2034,7 @@
         <v>19.48</v>
       </c>
     </row>
-    <row r="30" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>42879</v>
       </c>
@@ -2059,7 +2077,7 @@
         <v>21.16</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>42907</v>
       </c>
@@ -2096,7 +2114,7 @@
         <v>9.52</v>
       </c>
     </row>
-    <row r="32" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>42920</v>
       </c>
@@ -2142,7 +2160,7 @@
         <v>23.75</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>42956</v>
       </c>
@@ -2182,7 +2200,7 @@
         <v>9.09</v>
       </c>
     </row>
-    <row r="34" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>42991</v>
       </c>
@@ -2225,7 +2243,7 @@
         <v>23.24</v>
       </c>
     </row>
-    <row r="35" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>43033</v>
       </c>
@@ -2268,7 +2286,7 @@
         <v>21.64</v>
       </c>
     </row>
-    <row r="36" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>43061</v>
       </c>
@@ -2308,7 +2326,7 @@
         <v>16.080000000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>43117</v>
       </c>
@@ -2351,7 +2369,7 @@
         <v>22.16</v>
       </c>
     </row>
-    <row r="38" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>43152</v>
       </c>
@@ -2394,7 +2412,7 @@
         <v>17.28</v>
       </c>
     </row>
-    <row r="39" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>43181</v>
       </c>
@@ -2434,7 +2452,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>43216</v>
       </c>
@@ -2480,7 +2498,7 @@
         <v>21.85</v>
       </c>
     </row>
-    <row r="41" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>43244</v>
       </c>
@@ -2520,7 +2538,7 @@
         <v>13.080000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>43272</v>
       </c>
@@ -2563,7 +2581,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="43" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>43354</v>
       </c>
@@ -2603,7 +2621,7 @@
         <v>6.57</v>
       </c>
     </row>
-    <row r="44" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43384</v>
       </c>
@@ -2643,7 +2661,7 @@
         <v>16.350000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>43432</v>
       </c>
@@ -2683,7 +2701,7 @@
         <v>7.86</v>
       </c>
     </row>
-    <row r="46" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>43488</v>
       </c>
@@ -2726,7 +2744,7 @@
         <v>10.28</v>
       </c>
     </row>
-    <row r="47" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>43523</v>
       </c>
@@ -2769,7 +2787,7 @@
         <v>14.84</v>
       </c>
     </row>
-    <row r="48" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>43544</v>
       </c>
@@ -2812,7 +2830,7 @@
         <v>18.96</v>
       </c>
     </row>
-    <row r="49" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>43572</v>
       </c>
@@ -2848,11 +2866,11 @@
         <v>120</v>
       </c>
       <c r="P49" s="1">
-        <f t="shared" ref="P49:P62" si="2">SUM(H49:N49)*E49</f>
+        <f t="shared" ref="P49:P64" si="2">SUM(H49:N49)*E49</f>
         <v>9.69</v>
       </c>
     </row>
-    <row r="50" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="1" t="s">
         <v>121</v>
@@ -2885,7 +2903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>43628</v>
       </c>
@@ -2928,7 +2946,7 @@
         <v>21.84</v>
       </c>
     </row>
-    <row r="52" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>43663</v>
       </c>
@@ -2971,7 +2989,7 @@
         <v>15.76</v>
       </c>
     </row>
-    <row r="53" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>43705</v>
       </c>
@@ -3011,7 +3029,7 @@
         <v>12.299999999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>43726</v>
       </c>
@@ -3054,7 +3072,7 @@
         <v>13.84</v>
       </c>
     </row>
-    <row r="55" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>43754</v>
       </c>
@@ -3097,7 +3115,7 @@
         <v>14.16</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>43845</v>
       </c>
@@ -3137,7 +3155,7 @@
         <v>8.129999999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>43887</v>
       </c>
@@ -3180,7 +3198,7 @@
         <v>15.28</v>
       </c>
     </row>
-    <row r="58" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>44013</v>
       </c>
@@ -3215,7 +3233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>44062</v>
       </c>
@@ -3255,7 +3273,7 @@
         <v>10.11</v>
       </c>
     </row>
-    <row r="60" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>44097</v>
       </c>
@@ -3295,7 +3313,7 @@
         <v>12.419999999999998</v>
       </c>
     </row>
-    <row r="61" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>44307</v>
       </c>
@@ -3338,7 +3356,7 @@
         <v>6.88</v>
       </c>
     </row>
-    <row r="62" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>44335</v>
       </c>
@@ -3378,61 +3396,147 @@
         <v>6.99</v>
       </c>
     </row>
-    <row r="63" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A63" s="2"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-    </row>
-    <row r="64" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>44370</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E63" s="1">
+        <v>4.21</v>
+      </c>
+      <c r="F63" s="3">
+        <v>4.2106481481481488E-2</v>
+      </c>
+      <c r="G63" s="3">
+        <f>F63/E63</f>
+        <v>1.0001539544294891E-2</v>
+      </c>
+      <c r="H63" s="1">
+        <v>1</v>
+      </c>
+      <c r="I63" s="1">
+        <v>1</v>
+      </c>
+      <c r="J63" s="1">
+        <v>1</v>
+      </c>
+      <c r="N63" s="1">
+        <v>1</v>
+      </c>
+      <c r="O63" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="P63" s="1">
+        <f t="shared" si="2"/>
+        <v>16.84</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>44482</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="E64" s="1">
-        <f>SUM(E5:E62)</f>
-        <v>222.16</v>
+        <v>3.2</v>
+      </c>
+      <c r="F64" s="3">
+        <v>3.1261574074074074E-2</v>
       </c>
       <c r="G64" s="3">
-        <f>AVERAGE(G6:G62)</f>
-        <v>9.8620964241361853E-3</v>
+        <f>F64/E64</f>
+        <v>9.7692418981481476E-3</v>
       </c>
       <c r="H64" s="1">
-        <f>SUM(H5:H62)</f>
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="I64" s="1">
-        <f t="shared" ref="I64:M64" si="3">SUM(I5:I59)</f>
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="J64" s="1">
-        <f t="shared" si="3"/>
-        <v>49</v>
-      </c>
-      <c r="K64" s="1">
-        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="N64" s="1">
+        <v>1</v>
+      </c>
+      <c r="O64" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="P64" s="1">
+        <f t="shared" si="2"/>
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+      <c r="A65" s="2"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+    </row>
+    <row r="66" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+      <c r="E66" s="1">
+        <f>SUM(E5:E64)</f>
+        <v>229.57</v>
+      </c>
+      <c r="G66" s="3">
+        <f>AVERAGE(G6:G64)</f>
+        <v>9.8629137678935639E-3</v>
+      </c>
+      <c r="H66" s="1">
+        <f>SUM(H5:H64)</f>
+        <v>54</v>
+      </c>
+      <c r="I66" s="1">
+        <f>SUM(I5:I64)</f>
+        <v>38</v>
+      </c>
+      <c r="J66" s="1">
+        <f>SUM(J5:J64)</f>
+        <v>53</v>
+      </c>
+      <c r="K66" s="1">
+        <f t="shared" ref="I66:M66" si="3">SUM(K5:K59)</f>
         <v>0</v>
       </c>
-      <c r="L64" s="1">
+      <c r="L66" s="1">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="M64" s="1">
+      <c r="M66" s="1">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="N64" s="1">
-        <f>SUM(N5:N62)</f>
-        <v>53</v>
-      </c>
-      <c r="P64" s="1">
-        <f>SUM(P5:P63)</f>
-        <v>792.60000000000014</v>
-      </c>
-    </row>
-    <row r="67" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H67" s="1"/>
-      <c r="I67" s="1"/>
-      <c r="J67" s="6"/>
-      <c r="K67" s="6"/>
-      <c r="L67" s="6"/>
-      <c r="M67" s="6"/>
-      <c r="N67" s="6"/>
+      <c r="N66" s="1">
+        <f>SUM(N5:N64)</f>
+        <v>55</v>
+      </c>
+      <c r="P66" s="1">
+        <f>SUM(P5:P64)</f>
+        <v>822.24000000000012</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="6"/>
+      <c r="K69" s="6"/>
+      <c r="L69" s="6"/>
+      <c r="M69" s="6"/>
+      <c r="N69" s="6"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:L13">

</xml_diff>

<commit_message>
Added Bell and Harp
</commit_message>
<xml_diff>
--- a/pubrun.xlsx
+++ b/pubrun.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rich\Documents\root\home_and_family\fitness\pubrunner.github.io\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rich\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6CC024-A0B5-453B-8A82-A61475299A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F0F1BE-52EC-4955-AFE6-ABF564AD3EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="183">
   <si>
     <t>Stanley</t>
   </si>
@@ -573,6 +573,12 @@
   </si>
   <si>
     <t>Tar pits / Old kilns by A38?</t>
+  </si>
+  <si>
+    <t>The Bell and Harp</t>
+  </si>
+  <si>
+    <t>Barn owl, emus</t>
   </si>
 </sst>
 </file>
@@ -986,11 +992,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R69"/>
+  <dimension ref="A1:R70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3009,7 +3015,7 @@
         <v>120</v>
       </c>
       <c r="P47" s="1">
-        <f t="shared" ref="P47:P64" si="2">SUM(H47:N47)*E47</f>
+        <f t="shared" ref="P47:P65" si="2">SUM(H47:N47)*E47</f>
         <v>9.69</v>
       </c>
       <c r="Q47" s="1" t="s">
@@ -3408,7 +3414,7 @@
         <v>3.636574074074074E-2</v>
       </c>
       <c r="G57" s="3">
-        <f t="shared" ref="G57:G64" si="3">F57/E57</f>
+        <f t="shared" ref="G57:G65" si="3">F57/E57</f>
         <v>1.0791020991317726E-2</v>
       </c>
       <c r="H57" s="1">
@@ -3736,60 +3742,100 @@
       </c>
     </row>
     <row r="65" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="2"/>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
+      <c r="A65" s="2">
+        <v>44706</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E65" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="F65" s="3">
+        <v>2.9409722222222223E-2</v>
+      </c>
+      <c r="G65" s="3">
+        <f t="shared" si="3"/>
+        <v>1.1311431623931624E-2</v>
+      </c>
+      <c r="H65" s="1">
+        <v>1</v>
+      </c>
+      <c r="J65" s="1">
+        <v>1</v>
+      </c>
+      <c r="N65" s="1">
+        <v>1</v>
+      </c>
+      <c r="O65" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="P65" s="1">
+        <f t="shared" si="2"/>
+        <v>7.8000000000000007</v>
+      </c>
     </row>
     <row r="66" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
-      <c r="E66" s="1">
-        <f>SUM(E3:E64)</f>
-        <v>236.82</v>
-      </c>
-      <c r="G66" s="3">
-        <f>AVERAGE(G4:G64)</f>
-        <v>9.9072901023405727E-3</v>
-      </c>
-      <c r="H66" s="1">
-        <f t="shared" ref="H66:L66" si="4">SUM(H3:H64)</f>
-        <v>56</v>
-      </c>
-      <c r="I66" s="1">
-        <f t="shared" si="4"/>
+      <c r="A66" s="2"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+    </row>
+    <row r="67" spans="1:16" s="1" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+      <c r="E67" s="1">
+        <f>SUM(E3:E65)</f>
+        <v>239.42</v>
+      </c>
+      <c r="G67" s="3">
+        <f>AVERAGE(G4:G65)</f>
+        <v>9.9306924610337577E-3</v>
+      </c>
+      <c r="H67" s="1">
+        <f>SUM(H3:H65)</f>
+        <v>57</v>
+      </c>
+      <c r="I67" s="1">
+        <f t="shared" ref="H67:L67" si="4">SUM(I3:I64)</f>
         <v>40</v>
       </c>
-      <c r="J66" s="1">
+      <c r="J67" s="1">
         <f t="shared" si="4"/>
         <v>54</v>
       </c>
-      <c r="K66" s="1">
+      <c r="K67" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L66" s="1">
+      <c r="L67" s="1">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="M66" s="1">
+      <c r="M67" s="1">
         <f>SUM(M3:M64)</f>
         <v>4</v>
       </c>
-      <c r="N66" s="1">
-        <f>SUM(N3:N64)</f>
-        <v>57</v>
-      </c>
-      <c r="P66" s="1">
-        <f>SUM(P3:P64)</f>
-        <v>847.8900000000001</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
-      <c r="J69" s="5"/>
-      <c r="K69" s="5"/>
-      <c r="L69" s="5"/>
-      <c r="M69" s="5"/>
-      <c r="N69" s="5"/>
+      <c r="N67" s="1">
+        <f>SUM(N3:N65)</f>
+        <v>58</v>
+      </c>
+      <c r="P67" s="1">
+        <f>SUM(P3:P65)</f>
+        <v>855.69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="5"/>
+      <c r="K70" s="5"/>
+      <c r="L70" s="5"/>
+      <c r="M70" s="5"/>
+      <c r="N70" s="5"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L11">

</xml_diff>

<commit_message>
Added Darley Abbey run
</commit_message>
<xml_diff>
--- a/pubrun.xlsx
+++ b/pubrun.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rich/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D8DC68-3A62-1947-9CBC-96AFF9630CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A35340F-EB1C-6F4C-BAC7-6E82B0054ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2180" yWindow="1740" windowWidth="28060" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="222">
   <si>
     <t>Stanley</t>
   </si>
@@ -684,6 +684,18 @@
   </si>
   <si>
     <t>Multi-pub run, riverside drinks</t>
+  </si>
+  <si>
+    <t>The Abbey / The Furnace</t>
+  </si>
+  <si>
+    <t>start/end at pub + extra pub</t>
+  </si>
+  <si>
+    <t>The Abbey basement</t>
+  </si>
+  <si>
+    <t>Drunkard taxi drama, pint at The Furnace, talkative chap at the abbey, the summoning of Mr. McCoy!</t>
   </si>
 </sst>
 </file>
@@ -1065,9 +1077,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A79" sqref="A79"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P80" sqref="P80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2500,7 +2512,7 @@
         <v>92</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>15</v>
+        <v>219</v>
       </c>
       <c r="F34" s="1">
         <v>5.36</v>
@@ -3090,7 +3102,7 @@
         <v>120</v>
       </c>
       <c r="Q47" s="1">
-        <f t="shared" ref="Q47:Q78" si="2">SUM(I47:O47)*F47</f>
+        <f t="shared" ref="Q47:Q79" si="2">SUM(I47:O47)*F47</f>
         <v>9.69</v>
       </c>
       <c r="R47" s="1" t="s">
@@ -3230,7 +3242,7 @@
         <v>131</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>15</v>
+        <v>219</v>
       </c>
       <c r="F51" s="1">
         <v>4.0999999999999996</v>
@@ -3270,7 +3282,7 @@
         <v>40</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>15</v>
+        <v>219</v>
       </c>
       <c r="F52" s="1">
         <v>3.46</v>
@@ -3489,7 +3501,7 @@
         <v>3.636574074074074E-2</v>
       </c>
       <c r="H57" s="3">
-        <f t="shared" ref="H57:H78" si="3">G57/F57</f>
+        <f t="shared" ref="H57:H79" si="3">G57/F57</f>
         <v>1.0791020991317726E-2</v>
       </c>
       <c r="I57" s="1">
@@ -3692,7 +3704,7 @@
         <v>152</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>15</v>
+        <v>219</v>
       </c>
       <c r="F62" s="1">
         <v>3.2</v>
@@ -4043,7 +4055,7 @@
         <v>4.92</v>
       </c>
       <c r="F70" s="1">
-        <f t="shared" ref="F70:F78" si="4">E70*0.6213712</f>
+        <f t="shared" ref="F70:F79" si="4">E70*0.6213712</f>
         <v>3.0571463040000002</v>
       </c>
       <c r="G70" s="3">
@@ -4413,7 +4425,7 @@
         <v>6</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>15</v>
+        <v>219</v>
       </c>
       <c r="E78" s="1">
         <v>3.98</v>
@@ -4432,8 +4444,8 @@
       <c r="I78" s="1">
         <v>1</v>
       </c>
-      <c r="J78" s="1">
-        <v>1</v>
+      <c r="J78" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="K78" s="1">
         <v>1</v>
@@ -4446,16 +4458,64 @@
       </c>
       <c r="Q78" s="1">
         <f t="shared" si="2"/>
-        <v>9.8922295039999995</v>
+        <v>7.4191721279999996</v>
       </c>
       <c r="R78" s="1" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="79" spans="1:19" s="1" customFormat="1" ht="11" x14ac:dyDescent="0.15">
-      <c r="A79" s="2"/>
-      <c r="G79" s="3"/>
-      <c r="H79" s="3"/>
+      <c r="A79" s="2">
+        <v>45588</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E79" s="1">
+        <v>3.57</v>
+      </c>
+      <c r="F79" s="1">
+        <f t="shared" si="4"/>
+        <v>2.218295184</v>
+      </c>
+      <c r="G79" s="3">
+        <v>2.011574074074074E-2</v>
+      </c>
+      <c r="H79" s="3">
+        <f t="shared" si="3"/>
+        <v>9.0681081967046006E-3</v>
+      </c>
+      <c r="I79" s="1">
+        <v>1</v>
+      </c>
+      <c r="J79" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K79" s="1">
+        <v>1</v>
+      </c>
+      <c r="M79" s="1">
+        <v>1</v>
+      </c>
+      <c r="O79" s="1">
+        <v>1</v>
+      </c>
+      <c r="P79" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q79" s="1">
+        <f t="shared" si="2"/>
+        <v>8.8731807360000001</v>
+      </c>
+      <c r="R79" s="1" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="80" spans="1:19" s="1" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="A80" s="2"/>
@@ -4474,8 +4534,8 @@
     </row>
     <row r="83" spans="1:17" s="1" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="F83" s="1">
-        <f>SUM(F8:F78)</f>
-        <v>263.96478604800001</v>
+        <f>SUM(F8:F79)</f>
+        <v>266.18308123200001</v>
       </c>
       <c r="H83" s="3">
         <f>AVERAGE(H9:H73)</f>
@@ -4511,7 +4571,7 @@
       </c>
       <c r="Q83" s="1">
         <f>SUM(Q3:Q78)</f>
-        <v>987.92178214399996</v>
+        <v>985.44872476800003</v>
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">

</xml_diff>